<commit_message>
SubRes RESSOL og INDSOL får AFA = 1 igen
</commit_message>
<xml_diff>
--- a/TIMES-DE/SubRES_TMPL/SubRes_ELC_Techs_New.xlsx
+++ b/TIMES-DE/SubRES_TMPL/SubRes_ELC_Techs_New.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jonathan/Documents/GitHub/Bachelor_Git/TIMES-DE/SubRES_TMPL/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C9D300-F220-7A4E-9E78-F20E3F6BB4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="17016" windowHeight="12816" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="6" r:id="rId1"/>
@@ -70,7 +76,7 @@
     <definedName name="WasteCHP">[1]TechnologyData!$A$101:$M$129</definedName>
     <definedName name="Wood_SmallBP">[1]TechnologyData!$A$131:$M$158</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -85,13 +91,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Iben Moll Rasmussen</author>
     <author>Rikke Næraa</author>
   </authors>
   <commentList>
-    <comment ref="P5" authorId="0">
+    <comment ref="P5" authorId="0" shapeId="0" xr:uid="{429775CE-617E-40C7-839F-F070C3267782}">
       <text>
         <r>
           <rPr>
@@ -115,13 +121,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="W6" authorId="0">
+    <comment ref="W6" authorId="0" shapeId="0" xr:uid="{B8690188-748D-48FB-9BFA-DC3DF9DA3647}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -130,16 +136,25 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-What does this mean?</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>What does this mean?</t>
         </r>
       </text>
     </comment>
-    <comment ref="AF6" authorId="1">
+    <comment ref="AF6" authorId="1" shapeId="0" xr:uid="{B7412A02-F448-4F86-8542-023D849D13E6}">
       <text>
         <r>
           <rPr>
@@ -170,13 +185,13 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Iben Moll Rasmussen</author>
     <author>Rikke Næraa</author>
   </authors>
   <commentList>
-    <comment ref="P5" authorId="0">
+    <comment ref="P5" authorId="0" shapeId="0" xr:uid="{853A6447-1289-4B99-AD6E-5D9AB3CBFC7B}">
       <text>
         <r>
           <rPr>
@@ -200,7 +215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W6" authorId="0">
+    <comment ref="W6" authorId="0" shapeId="0" xr:uid="{E4287F17-6902-445F-959B-AFCDB3CC8014}">
       <text>
         <r>
           <rPr>
@@ -224,7 +239,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF6" authorId="1">
+    <comment ref="AF6" authorId="1" shapeId="0" xr:uid="{B853A64F-FF02-4A1A-A397-FE01B16FDE19}">
       <text>
         <r>
           <rPr>
@@ -1456,15 +1471,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="\Te\x\t"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1488,6 +1503,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1544,6 +1560,19 @@
     <font>
       <sz val="9"/>
       <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -1718,14 +1747,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1787,11 +1816,11 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="7" applyFill="1"/>
     <xf numFmtId="2" fontId="8" fillId="9" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="4" applyFill="1"/>
-    <xf numFmtId="166" fontId="8" fillId="9" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="8" fillId="9" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="6" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="166" fontId="8" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="8" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="11" borderId="0" xfId="4" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
@@ -1801,108 +1830,108 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="9" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="8" fillId="12" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="8" fillId="12" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="10" fillId="4" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="13" borderId="0" xfId="9" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="13" borderId="0" xfId="9" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="9" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
-    <cellStyle name="Comma 3 7" xfId="10"/>
-    <cellStyle name="Comma 3 8" xfId="8"/>
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+    <cellStyle name="Comma 3 7" xfId="10" xr:uid="{2C833FD2-D472-4EC9-A241-22328AC39DB6}"/>
+    <cellStyle name="Comma 3 8" xfId="8" xr:uid="{EEBC0FF0-D206-4A0E-B345-D80A997EC835}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 13 2" xfId="7"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 2 2" xfId="5"/>
-    <cellStyle name="Normal 3" xfId="2"/>
-    <cellStyle name="Normal 3 10" xfId="6"/>
-    <cellStyle name="Normal 4" xfId="4"/>
-    <cellStyle name="Normal 5" xfId="9"/>
-    <cellStyle name="Ugyldig" xfId="3" builtinId="27"/>
+    <cellStyle name="Normal 13 2" xfId="7" xr:uid="{C2F90FD3-72CA-4195-96F5-985134A4FC21}"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2 2" xfId="5" xr:uid="{1AC576CC-EE21-4631-8207-42C3281C3625}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 3 10" xfId="6" xr:uid="{3749CA24-9602-4138-8987-A6592B82EDD9}"/>
+    <cellStyle name="Normal 4" xfId="4" xr:uid="{861F0FED-FB99-47FD-9F3F-210480889B60}"/>
+    <cellStyle name="Normal 5" xfId="9" xr:uid="{D184B1FF-D706-4E5C-8643-993D534887E4}"/>
   </cellStyles>
   <dxfs count="22">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+      <numFmt numFmtId="164" formatCode="\Te\x\t"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+      <numFmt numFmtId="164" formatCode="\Te\x\t"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+      <numFmt numFmtId="164" formatCode="\Te\x\t"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+      <numFmt numFmtId="164" formatCode="\Te\x\t"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+      <numFmt numFmtId="164" formatCode="\Te\x\t"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+      <numFmt numFmtId="164" formatCode="\Te\x\t"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+      <numFmt numFmtId="164" formatCode="\Te\x\t"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+      <numFmt numFmtId="164" formatCode="\Te\x\t"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+      <numFmt numFmtId="164" formatCode="\Te\x\t"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+      <numFmt numFmtId="164" formatCode="\Te\x\t"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+      <numFmt numFmtId="164" formatCode="\Te\x\t"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+      <numFmt numFmtId="164" formatCode="\Te\x\t"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+      <numFmt numFmtId="164" formatCode="\Te\x\t"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+      <numFmt numFmtId="164" formatCode="\Te\x\t"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+      <numFmt numFmtId="164" formatCode="\Te\x\t"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+      <numFmt numFmtId="164" formatCode="\Te\x\t"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+      <numFmt numFmtId="164" formatCode="\Te\x\t"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+      <numFmt numFmtId="164" formatCode="\Te\x\t"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+      <numFmt numFmtId="164" formatCode="\Te\x\t"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+      <numFmt numFmtId="164" formatCode="\Te\x\t"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+      <numFmt numFmtId="164" formatCode="\Te\x\t"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -12522,130 +12551,130 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="B2:J25" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="B2:J25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table8" displayName="Table8" ref="B2:J25" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="B2:J25" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Csets" dataDxfId="19"/>
-    <tableColumn id="2" name="Region" dataDxfId="18"/>
-    <tableColumn id="3" name="CommName" dataDxfId="17"/>
-    <tableColumn id="4" name="CommDesc" dataDxfId="16"/>
-    <tableColumn id="5" name="Unit" dataDxfId="15"/>
-    <tableColumn id="6" name="LimType" dataDxfId="14"/>
-    <tableColumn id="7" name="CTSLvl" dataDxfId="13"/>
-    <tableColumn id="8" name="PeakTS" dataDxfId="12"/>
-    <tableColumn id="9" name="Ctype" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Csets" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Region" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="CommName" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="CommDesc" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Unit" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="LimType" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="CTSLvl" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="PeakTS" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Ctype" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="B2:I79" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="B2:I79"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table9" displayName="Table9" ref="B2:I79" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="B2:I79" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Sets" dataDxfId="8"/>
-    <tableColumn id="2" name="TechName" dataDxfId="7"/>
-    <tableColumn id="3" name="TechDesc" dataDxfId="6"/>
-    <tableColumn id="4" name="Tact" dataDxfId="5"/>
-    <tableColumn id="5" name="Tcap" dataDxfId="4"/>
-    <tableColumn id="6" name="Tslvl" dataDxfId="3"/>
-    <tableColumn id="7" name="PrimaryCG" dataDxfId="2"/>
-    <tableColumn id="8" name="Vintage" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Sets" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="TechName" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="TechDesc" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Tact" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Tcap" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Tslvl" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="PrimaryCG" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Vintage" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="B2:AM57" totalsRowShown="0">
-  <autoFilter ref="B2:AM57"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table10" displayName="Table10" ref="B2:AM57" totalsRowShown="0">
+  <autoFilter ref="B2:AM57" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="38">
-    <tableColumn id="1" name="TechName"/>
-    <tableColumn id="2" name="*TechDesc"/>
-    <tableColumn id="3" name="Comm-IN"/>
-    <tableColumn id="4" name="Comm-OUT"/>
-    <tableColumn id="5" name="CURR"/>
-    <tableColumn id="6" name="YEAR"/>
-    <tableColumn id="7" name="START"/>
-    <tableColumn id="8" name="EFF"/>
-    <tableColumn id="9" name="Share-I~FX~ELCC"/>
-    <tableColumn id="10" name="Share-I~FX~ELCSTM"/>
-    <tableColumn id="11" name="CHPR~UP"/>
-    <tableColumn id="12" name="CEH"/>
-    <tableColumn id="13" name="INVCOST"/>
-    <tableColumn id="14" name="FIXOM"/>
-    <tableColumn id="15" name="VAROM"/>
-    <tableColumn id="16" name="CAP2ACT"/>
-    <tableColumn id="17" name="AFA"/>
-    <tableColumn id="18" name="Peak"/>
-    <tableColumn id="19" name="LIFE"/>
-    <tableColumn id="20" name="ILED"/>
-    <tableColumn id="21" name="EMISSIONS~ELCNOX"/>
-    <tableColumn id="22" name="EMISSIONS~ELCCH4"/>
-    <tableColumn id="23" name="EMISSIONS~ELCN2O"/>
-    <tableColumn id="24" name="EMISSIONS~ELCSO2"/>
-    <tableColumn id="25" name="EMISSIONS~ELCPM"/>
-    <tableColumn id="26" name="*sheetNumber"/>
-    <tableColumn id="27" name="*sheetName"/>
-    <tableColumn id="28" name="*planttype"/>
-    <tableColumn id="29" name="*plantCategory"/>
-    <tableColumn id="30" name="*fuel_name"/>
-    <tableColumn id="31" name="*fuel_TIMES"/>
-    <tableColumn id="32" name="*dh_area"/>
-    <tableColumn id="33" name="*output"/>
-    <tableColumn id="34" name="*AFAforTrans"/>
-    <tableColumn id="35" name="*planttype_short"/>
-    <tableColumn id="36" name="*availability.pct"/>
-    <tableColumn id="37" name="*category"/>
-    <tableColumn id="38" name="*techNumber"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="TechName"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="*TechDesc"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Comm-IN"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Comm-OUT"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="CURR"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="YEAR"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="START"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="EFF"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Share-I~FX~ELCC"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Share-I~FX~ELCSTM"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="CHPR~UP"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="CEH"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="INVCOST"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="FIXOM"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="VAROM"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="CAP2ACT"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="AFA"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="Peak"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0200-000013000000}" name="LIFE"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0200-000014000000}" name="ILED"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0200-000015000000}" name="EMISSIONS~ELCNOX"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0200-000016000000}" name="EMISSIONS~ELCCH4"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0200-000017000000}" name="EMISSIONS~ELCN2O"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0200-000018000000}" name="EMISSIONS~ELCSO2"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0200-000019000000}" name="EMISSIONS~ELCPM"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0200-00001A000000}" name="*sheetNumber"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0200-00001B000000}" name="*sheetName"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0200-00001C000000}" name="*planttype"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0200-00001D000000}" name="*plantCategory"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0200-00001E000000}" name="*fuel_name"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0200-00001F000000}" name="*fuel_TIMES"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0200-000020000000}" name="*dh_area"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0200-000021000000}" name="*output"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0200-000022000000}" name="*AFAforTrans"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0200-000023000000}" name="*planttype_short"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0200-000024000000}" name="*availability.pct"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0200-000025000000}" name="*category"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0200-000026000000}" name="*techNumber"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="B2:AO138" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table11" displayName="Table11" ref="B2:AO138" totalsRowShown="0">
   <tableColumns count="40">
-    <tableColumn id="1" name="TechName"/>
-    <tableColumn id="2" name="*TechDesc"/>
-    <tableColumn id="3" name="Comm-IN"/>
-    <tableColumn id="4" name="Comm-OUT"/>
-    <tableColumn id="5" name="CURR"/>
-    <tableColumn id="6" name="YEAR"/>
-    <tableColumn id="7" name="START"/>
-    <tableColumn id="8" name="EFF"/>
-    <tableColumn id="9" name="Share-I~FX~ELCC"/>
-    <tableColumn id="10" name="Share-I~FX~ELCSTM"/>
-    <tableColumn id="39" name="CHPR~FX"/>
-    <tableColumn id="11" name="CHPR~UP"/>
-    <tableColumn id="12" name="CEH"/>
-    <tableColumn id="13" name="INVCOST"/>
-    <tableColumn id="14" name="FIXOM"/>
-    <tableColumn id="15" name="VAROM"/>
-    <tableColumn id="16" name="CAP2ACT"/>
-    <tableColumn id="17" name="AFA"/>
-    <tableColumn id="18" name="Peak"/>
-    <tableColumn id="19" name="LIFE"/>
-    <tableColumn id="20" name="ILED"/>
-    <tableColumn id="21" name="EMISSIONS~ELCNOX"/>
-    <tableColumn id="22" name="*EMISSIONS~ELCCH4"/>
-    <tableColumn id="23" name="EMISSIONS~ELCN2O"/>
-    <tableColumn id="24" name="EMISSIONS~ELCSO2"/>
-    <tableColumn id="25" name="EMISSIONS~ELCPM"/>
-    <tableColumn id="26" name="*sheetNumber"/>
-    <tableColumn id="27" name="*sheetName"/>
-    <tableColumn id="28" name="*planttype"/>
-    <tableColumn id="29" name="*plantCategory"/>
-    <tableColumn id="30" name="*fuel_name"/>
-    <tableColumn id="31" name="*fuel_TIMES"/>
-    <tableColumn id="32" name="*dh_area"/>
-    <tableColumn id="33" name="*output"/>
-    <tableColumn id="34" name="*AFAforTrans"/>
-    <tableColumn id="35" name="*planttype_short"/>
-    <tableColumn id="36" name="*availability.pct"/>
-    <tableColumn id="37" name="*category"/>
-    <tableColumn id="38" name="*techNumber"/>
-    <tableColumn id="40" name="EMISSIONS~ELCCH4" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="TechName"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="*TechDesc"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Comm-IN"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Comm-OUT"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="CURR"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="YEAR"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="START"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="EFF"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Share-I~FX~ELCC"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="Share-I~FX~ELCSTM"/>
+    <tableColumn id="39" xr3:uid="{3BE2BB3B-B102-4E4D-A636-66A9061ED3CC}" name="CHPR~FX"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="CHPR~UP"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="CEH"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0300-00000D000000}" name="INVCOST"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0300-00000E000000}" name="FIXOM"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0300-00000F000000}" name="VAROM"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0300-000010000000}" name="CAP2ACT"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0300-000011000000}" name="AFA"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0300-000012000000}" name="Peak"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0300-000013000000}" name="LIFE"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0300-000014000000}" name="ILED"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0300-000015000000}" name="EMISSIONS~ELCNOX"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0300-000016000000}" name="*EMISSIONS~ELCCH4"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0300-000017000000}" name="EMISSIONS~ELCN2O"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0300-000018000000}" name="EMISSIONS~ELCSO2"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0300-000019000000}" name="EMISSIONS~ELCPM"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0300-00001A000000}" name="*sheetNumber"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0300-00001B000000}" name="*sheetName"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0300-00001C000000}" name="*planttype"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0300-00001D000000}" name="*plantCategory"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0300-00001E000000}" name="*fuel_name"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0300-00001F000000}" name="*fuel_TIMES"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0300-000020000000}" name="*dh_area"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0300-000021000000}" name="*output"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0300-000022000000}" name="*AFAforTrans"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0300-000023000000}" name="*planttype_short"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0300-000024000000}" name="*availability.pct"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0300-000025000000}" name="*category"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0300-000026000000}" name="*techNumber"/>
+    <tableColumn id="40" xr3:uid="{8B7A128A-8967-4B89-9D3C-84BD0B4FF341}" name="EMISSIONS~ELCCH4" dataDxfId="0">
       <calculatedColumnFormula>Table11[[#This Row],[*EMISSIONS~ELCCH4]]/25</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -12654,48 +12683,48 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="B2:AN114" totalsRowShown="0">
-  <autoFilter ref="B2:AN114"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table12" displayName="Table12" ref="B2:AN114" totalsRowShown="0">
+  <autoFilter ref="B2:AN114" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
   <tableColumns count="39">
-    <tableColumn id="1" name="TechName"/>
-    <tableColumn id="2" name="*TechDesc"/>
-    <tableColumn id="3" name="Comm-IN"/>
-    <tableColumn id="4" name="Comm-OUT"/>
-    <tableColumn id="5" name="CURR"/>
-    <tableColumn id="6" name="YEAR"/>
-    <tableColumn id="7" name="START"/>
-    <tableColumn id="8" name="EFF"/>
-    <tableColumn id="9" name="Share-I~FX~ELCC"/>
-    <tableColumn id="10" name="Share-I~FX~ELCSTM"/>
-    <tableColumn id="39" name="CHPR~FX"/>
-    <tableColumn id="11" name="CHPR~UP"/>
-    <tableColumn id="12" name="CEH"/>
-    <tableColumn id="13" name="INVCOST"/>
-    <tableColumn id="14" name="FIXOM"/>
-    <tableColumn id="15" name="VAROM"/>
-    <tableColumn id="16" name="CAP2ACT"/>
-    <tableColumn id="17" name="AFA"/>
-    <tableColumn id="18" name="Peak"/>
-    <tableColumn id="19" name="LIFE"/>
-    <tableColumn id="20" name="ILED"/>
-    <tableColumn id="21" name="EMISSIONS~ELCNOX"/>
-    <tableColumn id="22" name="EMISSIONS~ELCCH4"/>
-    <tableColumn id="23" name="EMISSIONS~ELCN2O"/>
-    <tableColumn id="24" name="EMISSIONS~ELCSO2"/>
-    <tableColumn id="25" name="EMISSIONS~ELCPM"/>
-    <tableColumn id="26" name="*sheetNumber"/>
-    <tableColumn id="27" name="*sheetName"/>
-    <tableColumn id="28" name="*planttype"/>
-    <tableColumn id="29" name="*plantCategory"/>
-    <tableColumn id="30" name="*fuel_name"/>
-    <tableColumn id="31" name="*fuel_TIMES"/>
-    <tableColumn id="32" name="*dh_area"/>
-    <tableColumn id="33" name="*output"/>
-    <tableColumn id="34" name="*AFAforTrans"/>
-    <tableColumn id="35" name="*planttype_short"/>
-    <tableColumn id="36" name="*availability.pct"/>
-    <tableColumn id="37" name="*category"/>
-    <tableColumn id="38" name="*techNumber"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="TechName"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="*TechDesc"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Comm-IN"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Comm-OUT"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="CURR"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="YEAR"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="START"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="EFF"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="Share-I~FX~ELCC"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="Share-I~FX~ELCSTM"/>
+    <tableColumn id="39" xr3:uid="{12E94BB3-082E-4B27-993C-83A504C63817}" name="CHPR~FX"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="CHPR~UP"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0400-00000C000000}" name="CEH"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0400-00000D000000}" name="INVCOST"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0400-00000E000000}" name="FIXOM"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0400-00000F000000}" name="VAROM"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0400-000010000000}" name="CAP2ACT"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0400-000011000000}" name="AFA"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0400-000012000000}" name="Peak"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0400-000013000000}" name="LIFE"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0400-000014000000}" name="ILED"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0400-000015000000}" name="EMISSIONS~ELCNOX"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0400-000016000000}" name="EMISSIONS~ELCCH4"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0400-000017000000}" name="EMISSIONS~ELCN2O"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0400-000018000000}" name="EMISSIONS~ELCSO2"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0400-000019000000}" name="EMISSIONS~ELCPM"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0400-00001A000000}" name="*sheetNumber"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0400-00001B000000}" name="*sheetName"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0400-00001C000000}" name="*planttype"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0400-00001D000000}" name="*plantCategory"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0400-00001E000000}" name="*fuel_name"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0400-00001F000000}" name="*fuel_TIMES"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0400-000020000000}" name="*dh_area"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0400-000021000000}" name="*output"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0400-000022000000}" name="*AFAforTrans"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0400-000023000000}" name="*planttype_short"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0400-000024000000}" name="*availability.pct"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0400-000025000000}" name="*category"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0400-000026000000}" name="*techNumber"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12979,14 +13008,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -12994,19 +13023,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13019,7 +13048,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -13048,7 +13077,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
@@ -13067,7 +13096,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
@@ -13086,7 +13115,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
@@ -13105,7 +13134,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -13124,7 +13153,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
@@ -13143,7 +13172,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
@@ -13160,7 +13189,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
@@ -13177,7 +13206,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -13188,7 +13217,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -13199,7 +13228,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -13210,7 +13239,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -13221,7 +13250,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -13232,7 +13261,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -13243,7 +13272,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -13254,7 +13283,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -13265,7 +13294,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -13276,7 +13305,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -13287,7 +13316,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -13298,7 +13327,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -13309,7 +13338,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -13320,7 +13349,7 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -13331,7 +13360,7 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -13342,7 +13371,7 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -13363,20 +13392,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:I79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="53" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>38</v>
       </c>
@@ -13388,7 +13417,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>39</v>
       </c>
@@ -13414,7 +13443,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>72</v>
       </c>
@@ -13436,7 +13465,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>72</v>
       </c>
@@ -13458,7 +13487,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>72</v>
       </c>
@@ -13480,7 +13509,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>72</v>
       </c>
@@ -13502,7 +13531,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>72</v>
       </c>
@@ -13524,7 +13553,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>72</v>
       </c>
@@ -13546,7 +13575,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>72</v>
       </c>
@@ -13568,7 +13597,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>72</v>
       </c>
@@ -13590,7 +13619,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>72</v>
       </c>
@@ -13612,7 +13641,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>72</v>
       </c>
@@ -13634,7 +13663,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>72</v>
       </c>
@@ -13656,7 +13685,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>72</v>
       </c>
@@ -13678,7 +13707,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>72</v>
       </c>
@@ -13700,7 +13729,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>72</v>
       </c>
@@ -13722,7 +13751,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>72</v>
       </c>
@@ -13744,7 +13773,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>72</v>
       </c>
@@ -13766,7 +13795,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>72</v>
       </c>
@@ -13788,7 +13817,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>72</v>
       </c>
@@ -13810,7 +13839,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>72</v>
       </c>
@@ -13832,7 +13861,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>72</v>
       </c>
@@ -13854,7 +13883,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>72</v>
       </c>
@@ -13876,7 +13905,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>72</v>
       </c>
@@ -13898,7 +13927,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>72</v>
       </c>
@@ -13920,7 +13949,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>72</v>
       </c>
@@ -13942,7 +13971,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>72</v>
       </c>
@@ -13964,7 +13993,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>72</v>
       </c>
@@ -13986,7 +14015,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>72</v>
       </c>
@@ -14008,7 +14037,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>72</v>
       </c>
@@ -14030,7 +14059,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>72</v>
       </c>
@@ -14052,7 +14081,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>72</v>
       </c>
@@ -14074,7 +14103,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>72</v>
       </c>
@@ -14096,7 +14125,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>72</v>
       </c>
@@ -14118,7 +14147,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>72</v>
       </c>
@@ -14140,7 +14169,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>72</v>
       </c>
@@ -14162,7 +14191,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>72</v>
       </c>
@@ -14184,7 +14213,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>72</v>
       </c>
@@ -14206,7 +14235,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>72</v>
       </c>
@@ -14228,7 +14257,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>72</v>
       </c>
@@ -14250,7 +14279,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
         <v>47</v>
       </c>
@@ -14272,7 +14301,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>47</v>
       </c>
@@ -14294,7 +14323,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>47</v>
       </c>
@@ -14316,7 +14345,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
         <v>396</v>
       </c>
@@ -14338,7 +14367,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
         <v>47</v>
       </c>
@@ -14361,7 +14390,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
         <v>47</v>
       </c>
@@ -14384,7 +14413,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
         <v>47</v>
       </c>
@@ -14407,7 +14436,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
         <v>47</v>
       </c>
@@ -14430,7 +14459,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
         <v>47</v>
       </c>
@@ -14452,7 +14481,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
         <v>47</v>
       </c>
@@ -14474,7 +14503,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
         <v>47</v>
       </c>
@@ -14496,7 +14525,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
         <v>47</v>
       </c>
@@ -14518,7 +14547,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B53" s="1" t="s">
         <v>47</v>
       </c>
@@ -14540,7 +14569,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
         <v>95</v>
       </c>
@@ -14564,7 +14593,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" s="1" t="s">
         <v>95</v>
       </c>
@@ -14588,7 +14617,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B56" s="1" t="s">
         <v>95</v>
       </c>
@@ -14612,7 +14641,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B57" s="1" t="s">
         <v>95</v>
       </c>
@@ -14636,7 +14665,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B58" s="1" t="s">
         <v>95</v>
       </c>
@@ -14660,7 +14689,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B59" s="1" t="s">
         <v>95</v>
       </c>
@@ -14684,7 +14713,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B60" s="1" t="s">
         <v>95</v>
       </c>
@@ -14708,7 +14737,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B61" s="1" t="s">
         <v>95</v>
       </c>
@@ -14732,7 +14761,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B62" s="1" t="s">
         <v>95</v>
       </c>
@@ -14756,7 +14785,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B63" s="1" t="s">
         <v>95</v>
       </c>
@@ -14780,7 +14809,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B64" s="1" t="s">
         <v>95</v>
       </c>
@@ -14804,7 +14833,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B65" s="1" t="s">
         <v>95</v>
       </c>
@@ -14828,7 +14857,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B66" s="1" t="s">
         <v>95</v>
       </c>
@@ -14852,7 +14881,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
         <v>95</v>
       </c>
@@ -14876,7 +14905,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B68" s="1" t="s">
         <v>95</v>
       </c>
@@ -14900,7 +14929,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B69" s="1" t="s">
         <v>95</v>
       </c>
@@ -14924,7 +14953,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B70" s="1" t="s">
         <v>95</v>
       </c>
@@ -14948,7 +14977,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B71" s="1" t="s">
         <v>95</v>
       </c>
@@ -14972,7 +15001,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B72" s="1" t="s">
         <v>95</v>
       </c>
@@ -14996,7 +15025,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B73" s="1" t="s">
         <v>95</v>
       </c>
@@ -15020,7 +15049,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B74" s="1" t="s">
         <v>95</v>
       </c>
@@ -15044,7 +15073,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B75" s="1" t="s">
         <v>95</v>
       </c>
@@ -15068,7 +15097,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B76" s="1" t="s">
         <v>95</v>
       </c>
@@ -15092,7 +15121,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B77" s="1" t="s">
         <v>95</v>
       </c>
@@ -15116,7 +15145,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B78" s="1" t="s">
         <v>318</v>
       </c>
@@ -15138,7 +15167,7 @@
       <c r="H78" s="2"/>
       <c r="I78" s="1"/>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B79" s="1" t="s">
         <v>318</v>
       </c>
@@ -15170,25 +15199,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:AM57"/>
   <sheetViews>
     <sheetView topLeftCell="J1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+      <selection activeCell="AK2" sqref="AK2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:39" x14ac:dyDescent="0.2">
       <c r="G1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>40</v>
       </c>
@@ -15304,7 +15333,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>48</v>
       </c>
@@ -15393,7 +15422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F4" t="s">
         <v>320</v>
       </c>
@@ -15461,7 +15490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F5" t="s">
         <v>320</v>
       </c>
@@ -15529,7 +15558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F6" t="s">
         <v>320</v>
       </c>
@@ -15597,7 +15626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B7" s="56" t="s">
         <v>391</v>
       </c>
@@ -15680,7 +15709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F8" t="s">
         <v>320</v>
       </c>
@@ -15742,7 +15771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F9" t="s">
         <v>320</v>
       </c>
@@ -15804,7 +15833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F10" t="s">
         <v>320</v>
       </c>
@@ -15866,7 +15895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B11" s="56" t="s">
         <v>392</v>
       </c>
@@ -15952,7 +15981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F12" t="s">
         <v>320</v>
       </c>
@@ -16017,7 +16046,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F13" t="s">
         <v>320</v>
       </c>
@@ -16082,7 +16111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F14" t="s">
         <v>320</v>
       </c>
@@ -16147,7 +16176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F15" t="s">
         <v>320</v>
       </c>
@@ -16212,7 +16241,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>394</v>
       </c>
@@ -16298,7 +16327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F17" t="s">
         <v>320</v>
       </c>
@@ -16363,7 +16392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F18" t="s">
         <v>320</v>
       </c>
@@ -16428,7 +16457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F19" t="s">
         <v>320</v>
       </c>
@@ -16493,7 +16522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F20" t="s">
         <v>320</v>
       </c>
@@ -16558,7 +16587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>393</v>
       </c>
@@ -16644,7 +16673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F22" t="s">
         <v>320</v>
       </c>
@@ -16709,7 +16738,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F23" t="s">
         <v>320</v>
       </c>
@@ -16774,7 +16803,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F24" t="s">
         <v>320</v>
       </c>
@@ -16839,7 +16868,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F25" t="s">
         <v>320</v>
       </c>
@@ -16904,7 +16933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>56</v>
       </c>
@@ -16984,7 +17013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F27" t="s">
         <v>320</v>
       </c>
@@ -17043,7 +17072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F28" t="s">
         <v>320</v>
       </c>
@@ -17102,7 +17131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F29" t="s">
         <v>320</v>
       </c>
@@ -17161,7 +17190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>58</v>
       </c>
@@ -17241,7 +17270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F31" t="s">
         <v>320</v>
       </c>
@@ -17300,7 +17329,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F32" t="s">
         <v>320</v>
       </c>
@@ -17359,7 +17388,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F33" t="s">
         <v>320</v>
       </c>
@@ -17418,7 +17447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>60</v>
       </c>
@@ -17498,7 +17527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F35" t="s">
         <v>320</v>
       </c>
@@ -17557,7 +17586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F36" t="s">
         <v>320</v>
       </c>
@@ -17616,7 +17645,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F37" t="s">
         <v>320</v>
       </c>
@@ -17675,7 +17704,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>395</v>
       </c>
@@ -17758,7 +17787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>325</v>
       </c>
@@ -17823,7 +17852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>325</v>
       </c>
@@ -17888,7 +17917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>325</v>
       </c>
@@ -17953,7 +17982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>64</v>
       </c>
@@ -18054,7 +18083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F43" t="s">
         <v>320</v>
       </c>
@@ -18134,7 +18163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F44" t="s">
         <v>320</v>
       </c>
@@ -18214,7 +18243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F45" t="s">
         <v>320</v>
       </c>
@@ -18294,7 +18323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>66</v>
       </c>
@@ -18392,7 +18421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F47" t="s">
         <v>320</v>
       </c>
@@ -18469,7 +18498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F48" t="s">
         <v>320</v>
       </c>
@@ -18546,7 +18575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F49" t="s">
         <v>320</v>
       </c>
@@ -18623,7 +18652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>68</v>
       </c>
@@ -18721,7 +18750,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F51" t="s">
         <v>320</v>
       </c>
@@ -18798,7 +18827,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F52" t="s">
         <v>320</v>
       </c>
@@ -18875,7 +18904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F53" t="s">
         <v>320</v>
       </c>
@@ -18952,7 +18981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>70</v>
       </c>
@@ -19053,7 +19082,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F55" t="s">
         <v>320</v>
       </c>
@@ -19133,7 +19162,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F56" t="s">
         <v>320</v>
       </c>
@@ -19213,7 +19242,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:39" x14ac:dyDescent="0.2">
       <c r="F57" t="s">
         <v>320</v>
       </c>
@@ -19303,29 +19332,29 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:AO138"/>
   <sheetViews>
     <sheetView topLeftCell="O1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="AO3" sqref="AO3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:41" x14ac:dyDescent="0.2">
       <c r="G1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>40</v>
       </c>
@@ -19447,7 +19476,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>73</v>
       </c>
@@ -19555,7 +19584,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="4" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:41" x14ac:dyDescent="0.2">
       <c r="E4" t="s">
         <v>35</v>
       </c>
@@ -19645,7 +19674,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="5" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F5" t="s">
         <v>320</v>
       </c>
@@ -19732,7 +19761,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="6" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F6" t="s">
         <v>320</v>
       </c>
@@ -19819,7 +19848,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="7" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>75</v>
       </c>
@@ -19918,7 +19947,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="8" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:41" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
         <v>35</v>
       </c>
@@ -19999,7 +20028,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="9" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F9" t="s">
         <v>320</v>
       </c>
@@ -20077,7 +20106,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="10" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F10" t="s">
         <v>320</v>
       </c>
@@ -20155,7 +20184,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="11" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>77</v>
       </c>
@@ -20260,7 +20289,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="12" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:41" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
         <v>35</v>
       </c>
@@ -20347,7 +20376,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="13" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F13" t="s">
         <v>320</v>
       </c>
@@ -20431,7 +20460,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="14" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F14" t="s">
         <v>320</v>
       </c>
@@ -20515,7 +20544,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="15" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>79</v>
       </c>
@@ -20620,7 +20649,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="16" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:41" x14ac:dyDescent="0.2">
       <c r="E16" t="s">
         <v>35</v>
       </c>
@@ -20707,7 +20736,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="17" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F17" t="s">
         <v>320</v>
       </c>
@@ -20791,7 +20820,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="18" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F18" t="s">
         <v>320</v>
       </c>
@@ -20875,7 +20904,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="19" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>81</v>
       </c>
@@ -20980,7 +21009,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="20" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:41" x14ac:dyDescent="0.2">
       <c r="E20" t="s">
         <v>35</v>
       </c>
@@ -21067,7 +21096,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="21" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F21" t="s">
         <v>320</v>
       </c>
@@ -21151,7 +21180,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="22" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F22" t="s">
         <v>320</v>
       </c>
@@ -21235,7 +21264,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="23" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>83</v>
       </c>
@@ -21343,7 +21372,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="24" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:41" x14ac:dyDescent="0.2">
       <c r="E24" t="s">
         <v>35</v>
       </c>
@@ -21433,7 +21462,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="25" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F25" t="s">
         <v>320</v>
       </c>
@@ -21520,7 +21549,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="26" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F26" t="s">
         <v>320</v>
       </c>
@@ -21607,7 +21636,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="27" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>85</v>
       </c>
@@ -21709,7 +21738,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:41" x14ac:dyDescent="0.2">
       <c r="E28" t="s">
         <v>35</v>
       </c>
@@ -21793,7 +21822,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F29" t="s">
         <v>320</v>
       </c>
@@ -21874,7 +21903,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F30" t="s">
         <v>320</v>
       </c>
@@ -21955,7 +21984,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>87</v>
       </c>
@@ -22060,7 +22089,7 @@
         <v>12.6</v>
       </c>
     </row>
-    <row r="32" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:41" x14ac:dyDescent="0.2">
       <c r="E32" t="s">
         <v>35</v>
       </c>
@@ -22147,7 +22176,7 @@
         <v>12.6</v>
       </c>
     </row>
-    <row r="33" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F33" t="s">
         <v>320</v>
       </c>
@@ -22231,7 +22260,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="34" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F34" t="s">
         <v>320</v>
       </c>
@@ -22315,7 +22344,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>89</v>
       </c>
@@ -22426,7 +22455,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:41" x14ac:dyDescent="0.2">
       <c r="E36" t="s">
         <v>35</v>
       </c>
@@ -22519,7 +22548,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="37" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F37" t="s">
         <v>320</v>
       </c>
@@ -22609,7 +22638,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="38" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F38" t="s">
         <v>320</v>
       </c>
@@ -22699,7 +22728,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="39" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>91</v>
       </c>
@@ -22810,7 +22839,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="40" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:41" x14ac:dyDescent="0.2">
       <c r="E40" t="s">
         <v>35</v>
       </c>
@@ -22903,7 +22932,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="41" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F41" t="s">
         <v>320</v>
       </c>
@@ -22993,7 +23022,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="42" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F42" t="s">
         <v>320</v>
       </c>
@@ -23083,7 +23112,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="43" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>93</v>
       </c>
@@ -23194,7 +23223,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="44" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:41" x14ac:dyDescent="0.2">
       <c r="E44" t="s">
         <v>35</v>
       </c>
@@ -23287,7 +23316,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="45" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F45" t="s">
         <v>320</v>
       </c>
@@ -23377,7 +23406,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="46" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F46" t="s">
         <v>320</v>
       </c>
@@ -23467,7 +23496,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="47" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>96</v>
       </c>
@@ -23572,7 +23601,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="48" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F48" t="s">
         <v>320</v>
       </c>
@@ -23656,7 +23685,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="49" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F49" t="s">
         <v>320</v>
       </c>
@@ -23740,7 +23769,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="50" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F50" t="s">
         <v>320</v>
       </c>
@@ -23824,7 +23853,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="51" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>98</v>
       </c>
@@ -23929,7 +23958,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="52" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F52" t="s">
         <v>320</v>
       </c>
@@ -24013,7 +24042,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="53" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F53" t="s">
         <v>320</v>
       </c>
@@ -24097,7 +24126,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="54" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F54" t="s">
         <v>320</v>
       </c>
@@ -24181,7 +24210,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="55" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>100</v>
       </c>
@@ -24289,7 +24318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:41" x14ac:dyDescent="0.2">
       <c r="E56" t="s">
         <v>35</v>
       </c>
@@ -24379,7 +24408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F57" t="s">
         <v>320</v>
       </c>
@@ -24466,7 +24495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F58" t="s">
         <v>320</v>
       </c>
@@ -24553,7 +24582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>102</v>
       </c>
@@ -24661,7 +24690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:41" x14ac:dyDescent="0.2">
       <c r="E60" t="s">
         <v>35</v>
       </c>
@@ -24751,7 +24780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F61" t="s">
         <v>320</v>
       </c>
@@ -24838,7 +24867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F62" t="s">
         <v>320</v>
       </c>
@@ -24925,7 +24954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>104</v>
       </c>
@@ -25036,7 +25065,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="64" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:41" x14ac:dyDescent="0.2">
       <c r="E64" t="s">
         <v>35</v>
       </c>
@@ -25129,7 +25158,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="65" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F65" t="s">
         <v>320</v>
       </c>
@@ -25219,7 +25248,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="66" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F66" t="s">
         <v>320</v>
       </c>
@@ -25309,7 +25338,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="67" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>106</v>
       </c>
@@ -25414,7 +25443,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="68" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F68" t="s">
         <v>320</v>
       </c>
@@ -25498,7 +25527,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="69" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F69" t="s">
         <v>320</v>
       </c>
@@ -25582,7 +25611,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="70" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F70" t="s">
         <v>320</v>
       </c>
@@ -25666,7 +25695,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="71" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>108</v>
       </c>
@@ -25777,7 +25806,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="72" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:41" x14ac:dyDescent="0.2">
       <c r="E72" t="s">
         <v>35</v>
       </c>
@@ -25870,7 +25899,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="73" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F73" t="s">
         <v>320</v>
       </c>
@@ -25960,7 +25989,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="74" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F74" t="s">
         <v>320</v>
       </c>
@@ -26050,7 +26079,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="75" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>110</v>
       </c>
@@ -26161,7 +26190,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="76" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:41" x14ac:dyDescent="0.2">
       <c r="E76" t="s">
         <v>35</v>
       </c>
@@ -26254,7 +26283,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="77" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F77" t="s">
         <v>320</v>
       </c>
@@ -26344,7 +26373,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="78" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F78" t="s">
         <v>320</v>
       </c>
@@ -26434,7 +26463,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="79" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
         <v>112</v>
       </c>
@@ -26545,7 +26574,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="80" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:41" x14ac:dyDescent="0.2">
       <c r="E80" t="s">
         <v>35</v>
       </c>
@@ -26638,7 +26667,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="81" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F81" t="s">
         <v>320</v>
       </c>
@@ -26728,7 +26757,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="82" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F82" t="s">
         <v>320</v>
       </c>
@@ -26818,7 +26847,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="83" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>114</v>
       </c>
@@ -26920,7 +26949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F84" t="s">
         <v>320</v>
       </c>
@@ -27001,7 +27030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F85" t="s">
         <v>320</v>
       </c>
@@ -27082,7 +27111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F86" t="s">
         <v>320</v>
       </c>
@@ -27163,7 +27192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>116</v>
       </c>
@@ -27271,7 +27300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:41" x14ac:dyDescent="0.2">
       <c r="E88" t="s">
         <v>35</v>
       </c>
@@ -27361,7 +27390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F89" t="s">
         <v>320</v>
       </c>
@@ -27448,7 +27477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F90" t="s">
         <v>320</v>
       </c>
@@ -27535,7 +27564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>118</v>
       </c>
@@ -27643,7 +27672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:41" x14ac:dyDescent="0.2">
       <c r="E92" t="s">
         <v>35</v>
       </c>
@@ -27733,7 +27762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F93" t="s">
         <v>320</v>
       </c>
@@ -27820,7 +27849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F94" t="s">
         <v>320</v>
       </c>
@@ -27907,7 +27936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
         <v>120</v>
       </c>
@@ -28015,7 +28044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:41" x14ac:dyDescent="0.2">
       <c r="E96" t="s">
         <v>35</v>
       </c>
@@ -28105,7 +28134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F97" t="s">
         <v>320</v>
       </c>
@@ -28192,7 +28221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F98" t="s">
         <v>320</v>
       </c>
@@ -28279,7 +28308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
         <v>122</v>
       </c>
@@ -28372,7 +28401,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="100" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:41" x14ac:dyDescent="0.2">
       <c r="E100" t="s">
         <v>35</v>
       </c>
@@ -28447,7 +28476,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="101" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F101" t="s">
         <v>320</v>
       </c>
@@ -28519,7 +28548,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="102" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F102" t="s">
         <v>320</v>
       </c>
@@ -28591,7 +28620,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="103" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>124</v>
       </c>
@@ -28681,7 +28710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:41" x14ac:dyDescent="0.2">
       <c r="E104" t="s">
         <v>35</v>
       </c>
@@ -28753,7 +28782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F105" t="s">
         <v>320</v>
       </c>
@@ -28822,7 +28851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F106" t="s">
         <v>320</v>
       </c>
@@ -28891,7 +28920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
         <v>126</v>
       </c>
@@ -28981,7 +29010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:41" x14ac:dyDescent="0.2">
       <c r="D108" t="s">
         <v>28</v>
       </c>
@@ -29053,7 +29082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:41" x14ac:dyDescent="0.2">
       <c r="D109" t="s">
         <v>22</v>
       </c>
@@ -29125,7 +29154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F110" t="s">
         <v>320</v>
       </c>
@@ -29194,7 +29223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
         <v>128</v>
       </c>
@@ -29284,7 +29313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:41" x14ac:dyDescent="0.2">
       <c r="D112" t="s">
         <v>22</v>
       </c>
@@ -29356,7 +29385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F113" t="s">
         <v>320</v>
       </c>
@@ -29425,7 +29454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F114" t="s">
         <v>320</v>
       </c>
@@ -29494,7 +29523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
         <v>130</v>
       </c>
@@ -29584,7 +29613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F116" t="s">
         <v>320</v>
       </c>
@@ -29653,7 +29682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F117" t="s">
         <v>320</v>
       </c>
@@ -29722,7 +29751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F118" t="s">
         <v>320</v>
       </c>
@@ -29791,7 +29820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
         <v>132</v>
       </c>
@@ -29893,7 +29922,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="120" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F120" t="s">
         <v>320</v>
       </c>
@@ -29974,7 +30003,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="121" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F121" t="s">
         <v>320</v>
       </c>
@@ -30055,7 +30084,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="122" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F122" t="s">
         <v>320</v>
       </c>
@@ -30136,7 +30165,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="123" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
         <v>134</v>
       </c>
@@ -30232,7 +30261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:41" x14ac:dyDescent="0.2">
       <c r="D124" t="s">
         <v>28</v>
       </c>
@@ -30310,7 +30339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:41" x14ac:dyDescent="0.2">
       <c r="D125" t="s">
         <v>22</v>
       </c>
@@ -30388,7 +30417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F126" t="s">
         <v>320</v>
       </c>
@@ -30463,7 +30492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B127" t="s">
         <v>136</v>
       </c>
@@ -30559,7 +30588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:41" x14ac:dyDescent="0.2">
       <c r="D128" t="s">
         <v>28</v>
       </c>
@@ -30637,7 +30666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:41" x14ac:dyDescent="0.2">
       <c r="D129" t="s">
         <v>22</v>
       </c>
@@ -30715,7 +30744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F130" t="s">
         <v>320</v>
       </c>
@@ -30790,7 +30819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
         <v>138</v>
       </c>
@@ -30886,7 +30915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:41" x14ac:dyDescent="0.2">
       <c r="D132" t="s">
         <v>22</v>
       </c>
@@ -30964,7 +30993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F133" t="s">
         <v>320</v>
       </c>
@@ -31039,7 +31068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F134" t="s">
         <v>320</v>
       </c>
@@ -31114,7 +31143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
         <v>140</v>
       </c>
@@ -31204,7 +31233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F136" t="s">
         <v>320</v>
       </c>
@@ -31273,7 +31302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F137" t="s">
         <v>320</v>
       </c>
@@ -31342,7 +31371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:41" x14ac:dyDescent="0.2">
       <c r="F138" t="s">
         <v>320</v>
       </c>
@@ -31421,24 +31450,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:AN114"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:40" x14ac:dyDescent="0.2">
       <c r="G1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>40</v>
       </c>
@@ -31557,7 +31586,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B3" s="57" t="s">
         <v>142</v>
       </c>
@@ -31652,7 +31681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B4" s="57"/>
       <c r="E4" t="s">
         <v>37</v>
@@ -31730,7 +31759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B5" s="57"/>
       <c r="F5" t="s">
         <v>320</v>
@@ -31805,7 +31834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B6" s="57"/>
       <c r="F6" t="s">
         <v>320</v>
@@ -31880,7 +31909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B7" s="57" t="s">
         <v>143</v>
       </c>
@@ -31981,7 +32010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B8" s="57"/>
       <c r="E8" t="s">
         <v>37</v>
@@ -32065,7 +32094,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B9" s="57"/>
       <c r="F9" t="s">
         <v>320</v>
@@ -32146,7 +32175,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B10" s="57"/>
       <c r="F10" t="s">
         <v>320</v>
@@ -32227,7 +32256,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B11" s="57" t="s">
         <v>144</v>
       </c>
@@ -32328,7 +32357,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B12" s="57"/>
       <c r="E12" t="s">
         <v>37</v>
@@ -32412,7 +32441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B13" s="57"/>
       <c r="F13" t="s">
         <v>320</v>
@@ -32493,7 +32522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B14" s="57"/>
       <c r="F14" t="s">
         <v>320</v>
@@ -32574,7 +32603,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B15" s="57" t="s">
         <v>145</v>
       </c>
@@ -32678,7 +32707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B16" s="57"/>
       <c r="E16" t="s">
         <v>37</v>
@@ -32765,7 +32794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B17" s="57"/>
       <c r="F17" t="s">
         <v>320</v>
@@ -32849,7 +32878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B18" s="57"/>
       <c r="F18" t="s">
         <v>320</v>
@@ -32933,7 +32962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B19" s="57" t="s">
         <v>146</v>
       </c>
@@ -33031,7 +33060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B20" s="57"/>
       <c r="E20" t="s">
         <v>37</v>
@@ -33112,7 +33141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B21" s="57"/>
       <c r="F21" t="s">
         <v>320</v>
@@ -33190,7 +33219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B22" s="57"/>
       <c r="F22" t="s">
         <v>320</v>
@@ -33268,7 +33297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B23" s="57" t="s">
         <v>147</v>
       </c>
@@ -33369,7 +33398,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B24" s="57"/>
       <c r="E24" t="s">
         <v>37</v>
@@ -33453,7 +33482,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B25" s="57"/>
       <c r="F25" t="s">
         <v>320</v>
@@ -33534,7 +33563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B26" s="57"/>
       <c r="F26" t="s">
         <v>320</v>
@@ -33615,7 +33644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B27" s="57" t="s">
         <v>148</v>
       </c>
@@ -33722,7 +33751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B28" s="57"/>
       <c r="E28" t="s">
         <v>37</v>
@@ -33812,7 +33841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B29" s="57"/>
       <c r="F29" t="s">
         <v>320</v>
@@ -33899,7 +33928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B30" s="57"/>
       <c r="F30" t="s">
         <v>320</v>
@@ -33986,7 +34015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B31" s="57" t="s">
         <v>149</v>
       </c>
@@ -34093,7 +34122,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B32" s="57"/>
       <c r="E32" t="s">
         <v>37</v>
@@ -34183,7 +34212,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B33" s="57"/>
       <c r="F33" t="s">
         <v>320</v>
@@ -34270,7 +34299,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B34" s="57"/>
       <c r="F34" t="s">
         <v>320</v>
@@ -34357,7 +34386,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B35" s="57" t="s">
         <v>150</v>
       </c>
@@ -34458,7 +34487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B36" s="57"/>
       <c r="F36" t="s">
         <v>320</v>
@@ -34539,7 +34568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B37" s="57"/>
       <c r="F37" t="s">
         <v>320</v>
@@ -34620,7 +34649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B38" s="57"/>
       <c r="F38" t="s">
         <v>320</v>
@@ -34701,7 +34730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B39" s="57" t="s">
         <v>151</v>
       </c>
@@ -34802,7 +34831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B40" s="57"/>
       <c r="F40" t="s">
         <v>320</v>
@@ -34883,7 +34912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B41" s="57"/>
       <c r="F41" t="s">
         <v>320</v>
@@ -34964,7 +34993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B42" s="57"/>
       <c r="F42" t="s">
         <v>320</v>
@@ -35045,7 +35074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B43" s="57" t="s">
         <v>152</v>
       </c>
@@ -35149,7 +35178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B44" s="57"/>
       <c r="E44" t="s">
         <v>37</v>
@@ -35236,7 +35265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B45" s="57"/>
       <c r="F45" t="s">
         <v>320</v>
@@ -35320,7 +35349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B46" s="57"/>
       <c r="F46" t="s">
         <v>320</v>
@@ -35404,7 +35433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B47" s="57" t="s">
         <v>153</v>
       </c>
@@ -35511,7 +35540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B48" s="57"/>
       <c r="E48" t="s">
         <v>37</v>
@@ -35601,7 +35630,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B49" s="57"/>
       <c r="F49" t="s">
         <v>320</v>
@@ -35688,7 +35717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B50" s="57"/>
       <c r="F50" t="s">
         <v>320</v>
@@ -35775,7 +35804,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B51" s="57" t="s">
         <v>154</v>
       </c>
@@ -35876,7 +35905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B52" s="57"/>
       <c r="F52" t="s">
         <v>320</v>
@@ -35957,7 +35986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B53" s="57"/>
       <c r="F53" t="s">
         <v>320</v>
@@ -36038,7 +36067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B54" s="57"/>
       <c r="F54" t="s">
         <v>320</v>
@@ -36119,7 +36148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B55" s="57" t="s">
         <v>155</v>
       </c>
@@ -36226,7 +36255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B56" s="57"/>
       <c r="E56" t="s">
         <v>37</v>
@@ -36316,7 +36345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B57" s="57"/>
       <c r="F57" t="s">
         <v>320</v>
@@ -36403,7 +36432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B58" s="57"/>
       <c r="F58" t="s">
         <v>320</v>
@@ -36490,7 +36519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B59" s="57" t="s">
         <v>156</v>
       </c>
@@ -36597,7 +36626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B60" s="57"/>
       <c r="E60" t="s">
         <v>37</v>
@@ -36687,7 +36716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B61" s="57"/>
       <c r="F61" t="s">
         <v>320</v>
@@ -36774,7 +36803,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B62" s="57"/>
       <c r="F62" t="s">
         <v>320</v>
@@ -36861,7 +36890,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B63" s="57" t="s">
         <v>157</v>
       </c>
@@ -36959,7 +36988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B64" s="57"/>
       <c r="F64" t="s">
         <v>320</v>
@@ -37037,7 +37066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B65" s="57"/>
       <c r="F65" t="s">
         <v>320</v>
@@ -37115,7 +37144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B66" s="57"/>
       <c r="F66" t="s">
         <v>320</v>
@@ -37193,7 +37222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B67" s="57" t="s">
         <v>158</v>
       </c>
@@ -37297,7 +37326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B68" s="57"/>
       <c r="E68" t="s">
         <v>37</v>
@@ -37384,7 +37413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B69" s="57"/>
       <c r="F69" t="s">
         <v>320</v>
@@ -37468,7 +37497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B70" s="57"/>
       <c r="F70" t="s">
         <v>320</v>
@@ -37552,7 +37581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B71" s="57" t="s">
         <v>159</v>
       </c>
@@ -37656,7 +37685,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B72" s="57"/>
       <c r="E72" t="s">
         <v>37</v>
@@ -37743,7 +37772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B73" s="57"/>
       <c r="F73" t="s">
         <v>320</v>
@@ -37827,7 +37856,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B74" s="57"/>
       <c r="F74" t="s">
         <v>320</v>
@@ -37911,7 +37940,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B75" s="57" t="s">
         <v>160</v>
       </c>
@@ -37997,7 +38026,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B76" s="57"/>
       <c r="E76" t="s">
         <v>37</v>
@@ -38069,7 +38098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B77" s="57"/>
       <c r="F77" t="s">
         <v>320</v>
@@ -38138,7 +38167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B78" s="57"/>
       <c r="F78" t="s">
         <v>320</v>
@@ -38207,7 +38236,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B79" s="57" t="s">
         <v>161</v>
       </c>
@@ -38290,7 +38319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B80" s="57"/>
       <c r="E80" t="s">
         <v>37</v>
@@ -38359,7 +38388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:40" x14ac:dyDescent="0.2">
       <c r="F81" t="s">
         <v>320</v>
       </c>
@@ -38424,7 +38453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:40" x14ac:dyDescent="0.2">
       <c r="F82" t="s">
         <v>320</v>
       </c>
@@ -38489,7 +38518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>162</v>
       </c>
@@ -38575,7 +38604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:40" x14ac:dyDescent="0.2">
       <c r="D84" t="s">
         <v>28</v>
       </c>
@@ -38643,7 +38672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:40" x14ac:dyDescent="0.2">
       <c r="D85" t="s">
         <v>22</v>
       </c>
@@ -38711,7 +38740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:40" x14ac:dyDescent="0.2">
       <c r="F86" t="s">
         <v>320</v>
       </c>
@@ -38776,7 +38805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>163</v>
       </c>
@@ -38862,7 +38891,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:40" x14ac:dyDescent="0.2">
       <c r="D88" t="s">
         <v>22</v>
       </c>
@@ -38930,7 +38959,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:40" x14ac:dyDescent="0.2">
       <c r="F89" t="s">
         <v>320</v>
       </c>
@@ -38995,7 +39024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:40" x14ac:dyDescent="0.2">
       <c r="F90" t="s">
         <v>320</v>
       </c>
@@ -39060,7 +39089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>164</v>
       </c>
@@ -39146,7 +39175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:40" x14ac:dyDescent="0.2">
       <c r="F92" t="s">
         <v>320</v>
       </c>
@@ -39211,7 +39240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:40" x14ac:dyDescent="0.2">
       <c r="F93" t="s">
         <v>320</v>
       </c>
@@ -39276,7 +39305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:40" x14ac:dyDescent="0.2">
       <c r="F94" t="s">
         <v>320</v>
       </c>
@@ -39341,7 +39370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
         <v>165</v>
       </c>
@@ -39439,7 +39468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:40" x14ac:dyDescent="0.2">
       <c r="F96" t="s">
         <v>320</v>
       </c>
@@ -39516,7 +39545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:40" x14ac:dyDescent="0.2">
       <c r="F97" t="s">
         <v>320</v>
       </c>
@@ -39593,7 +39622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:40" x14ac:dyDescent="0.2">
       <c r="F98" t="s">
         <v>320</v>
       </c>
@@ -39670,7 +39699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
         <v>166</v>
       </c>
@@ -39762,7 +39791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:40" x14ac:dyDescent="0.2">
       <c r="D100" t="s">
         <v>28</v>
       </c>
@@ -39836,7 +39865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:40" x14ac:dyDescent="0.2">
       <c r="D101" t="s">
         <v>22</v>
       </c>
@@ -39910,7 +39939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:40" x14ac:dyDescent="0.2">
       <c r="F102" t="s">
         <v>320</v>
       </c>
@@ -39981,7 +40010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>167</v>
       </c>
@@ -40073,7 +40102,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:40" x14ac:dyDescent="0.2">
       <c r="D104" t="s">
         <v>28</v>
       </c>
@@ -40147,7 +40176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:40" x14ac:dyDescent="0.2">
       <c r="D105" t="s">
         <v>22</v>
       </c>
@@ -40221,7 +40250,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:40" x14ac:dyDescent="0.2">
       <c r="F106" t="s">
         <v>320</v>
       </c>
@@ -40292,7 +40321,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
         <v>168</v>
       </c>
@@ -40384,7 +40413,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:40" x14ac:dyDescent="0.2">
       <c r="D108" t="s">
         <v>22</v>
       </c>
@@ -40458,7 +40487,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:40" x14ac:dyDescent="0.2">
       <c r="F109" t="s">
         <v>320</v>
       </c>
@@ -40529,7 +40558,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:40" x14ac:dyDescent="0.2">
       <c r="F110" t="s">
         <v>320</v>
       </c>
@@ -40600,7 +40629,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
         <v>169</v>
       </c>
@@ -40686,7 +40715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:40" x14ac:dyDescent="0.2">
       <c r="F112" t="s">
         <v>320</v>
       </c>
@@ -40751,7 +40780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="6:40" x14ac:dyDescent="0.3">
+    <row r="113" spans="6:40" x14ac:dyDescent="0.2">
       <c r="F113" t="s">
         <v>320</v>
       </c>
@@ -40816,7 +40845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="6:40" x14ac:dyDescent="0.3">
+    <row r="114" spans="6:40" x14ac:dyDescent="0.2">
       <c r="F114" t="s">
         <v>320</v>
       </c>
@@ -40891,31 +40920,33 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6445A955-CCF8-4BF0-957D-836863B7171B}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
   <dimension ref="A3:AQ20"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="X19" sqref="X19"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="3"/>
+    <col min="2" max="2" width="39.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="31" width="9.1640625" style="3"/>
+    <col min="32" max="32" width="17.6640625" style="3" customWidth="1"/>
+    <col min="33" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
       <c r="F3" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:43" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:43" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>40</v>
       </c>
@@ -41020,7 +41051,7 @@
       <c r="AO4" s="10"/>
       <c r="AP4" s="10"/>
     </row>
-    <row r="5" spans="1:43" s="14" customFormat="1" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:43" s="14" customFormat="1" ht="81.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>330</v>
       </c>
@@ -41122,7 +41153,7 @@
       <c r="AO5" s="15"/>
       <c r="AP5" s="15"/>
     </row>
-    <row r="6" spans="1:43" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:43" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>355</v>
       </c>
@@ -41208,7 +41239,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="str">
         <f>C20</f>
         <v>INDSOLPV5N</v>
@@ -41260,9 +41291,7 @@
         <f>3.6*8760/1000000</f>
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="X7" s="26">
-        <v>0.05</v>
-      </c>
+      <c r="X7" s="26"/>
       <c r="Y7" s="30">
         <v>0.26</v>
       </c>
@@ -41304,7 +41333,7 @@
         <v>1024.1119531500001</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A8" s="23"/>
       <c r="B8" s="24"/>
       <c r="C8" s="23"/>
@@ -41330,9 +41359,7 @@
       <c r="U8" s="28"/>
       <c r="V8" s="28"/>
       <c r="W8" s="29"/>
-      <c r="X8" s="26">
-        <v>0.05</v>
-      </c>
+      <c r="X8" s="26"/>
       <c r="Y8" s="30"/>
       <c r="Z8" s="31"/>
       <c r="AA8" s="28"/>
@@ -41353,7 +41380,7 @@
       <c r="AP8" s="27"/>
       <c r="AQ8" s="38"/>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A9" s="23"/>
       <c r="B9" s="24"/>
       <c r="C9" s="23"/>
@@ -41393,9 +41420,7 @@
         <f>3.6*8760/1000000</f>
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="X9" s="26">
-        <v>0.05</v>
-      </c>
+      <c r="X9" s="41"/>
       <c r="Y9" s="30">
         <v>0.26</v>
       </c>
@@ -41433,7 +41458,7 @@
         <v>1106.1124824750002</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A10" s="23"/>
       <c r="B10" s="24"/>
       <c r="C10" s="23"/>
@@ -41473,9 +41498,7 @@
         <f>3.6*8760/1000000</f>
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="X10" s="26">
-        <v>0.05</v>
-      </c>
+      <c r="X10" s="41"/>
       <c r="Y10" s="30">
         <v>0.26</v>
       </c>
@@ -41513,7 +41536,7 @@
         <v>1142.0167253550001</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A11" s="23"/>
       <c r="B11" s="24"/>
       <c r="C11" s="23"/>
@@ -41553,9 +41576,7 @@
         <f>3.6*8760/1000000</f>
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="X11" s="26">
-        <v>0.05</v>
-      </c>
+      <c r="X11" s="41"/>
       <c r="Y11" s="30">
         <v>0.26</v>
       </c>
@@ -41593,7 +41614,7 @@
         <v>1178.4496977000001</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="47" t="s">
         <v>38</v>
       </c>
@@ -41605,7 +41626,7 @@
       <c r="H17" s="48"/>
       <c r="I17" s="48"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="49" t="s">
         <v>39</v>
       </c>
@@ -41631,7 +41652,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" ht="64" x14ac:dyDescent="0.2">
       <c r="B19" s="50" t="s">
         <v>377</v>
       </c>
@@ -41657,7 +41678,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="51" t="s">
         <v>47</v>
       </c>
@@ -41686,31 +41707,31 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3577ED8-9856-45D0-AE86-3713751A8512}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
   <dimension ref="A3:AQ20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7:X12"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="3"/>
+    <col min="4" max="4" width="39.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
       <c r="F3" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:43" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:43" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>40</v>
       </c>
@@ -41815,7 +41836,7 @@
       <c r="AO4" s="10"/>
       <c r="AP4" s="10"/>
     </row>
-    <row r="5" spans="1:43" s="14" customFormat="1" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:43" s="14" customFormat="1" ht="81.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>330</v>
       </c>
@@ -41917,7 +41938,7 @@
       <c r="AO5" s="15"/>
       <c r="AP5" s="15"/>
     </row>
-    <row r="6" spans="1:43" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:43" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>355</v>
       </c>
@@ -42003,7 +42024,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="str">
         <f>C20</f>
         <v>RESSOLPV5N</v>
@@ -42055,9 +42076,7 @@
         <f>3.6*8760/1000000</f>
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="X7" s="26">
-        <v>0.05</v>
-      </c>
+      <c r="X7" s="26"/>
       <c r="Y7" s="30">
         <v>0.26</v>
       </c>
@@ -42099,7 +42118,7 @@
         <v>961.2395735250002</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -42125,9 +42144,7 @@
       <c r="U8" s="28"/>
       <c r="V8" s="28"/>
       <c r="W8" s="29"/>
-      <c r="X8" s="26">
-        <v>0.05</v>
-      </c>
+      <c r="X8" s="26"/>
       <c r="Y8" s="30"/>
       <c r="Z8" s="31"/>
       <c r="AA8" s="28"/>
@@ -42148,7 +42165,7 @@
       <c r="AP8" s="27"/>
       <c r="AQ8" s="54"/>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A9" s="23"/>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
@@ -42174,9 +42191,7 @@
       <c r="U9" s="28"/>
       <c r="V9" s="28"/>
       <c r="W9" s="29"/>
-      <c r="X9" s="26">
-        <v>0.05</v>
-      </c>
+      <c r="X9" s="26"/>
       <c r="Y9" s="30"/>
       <c r="Z9" s="31"/>
       <c r="AA9" s="28"/>
@@ -42197,7 +42212,7 @@
       <c r="AP9" s="27"/>
       <c r="AQ9" s="54"/>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A10" s="23"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
@@ -42237,9 +42252,7 @@
         <f>3.6*8760/1000000</f>
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="X10" s="26">
-        <v>0.05</v>
-      </c>
+      <c r="X10" s="41"/>
       <c r="Y10" s="30">
         <v>0.26</v>
       </c>
@@ -42277,7 +42290,7 @@
         <v>1021.0269069000002</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A11" s="23"/>
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
@@ -42317,9 +42330,7 @@
         <f>3.6*8760/1000000</f>
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="X11" s="26">
-        <v>0.05</v>
-      </c>
+      <c r="X11" s="41"/>
       <c r="Y11" s="30">
         <v>0.26</v>
       </c>
@@ -42358,7 +42369,7 @@
         <v>1054.9421363250001</v>
       </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A12" s="23"/>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
@@ -42398,9 +42409,7 @@
         <f>3.6*8760/1000000</f>
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="X12" s="26">
-        <v>0.05</v>
-      </c>
+      <c r="X12" s="41"/>
       <c r="Y12" s="30">
         <v>0.26</v>
       </c>
@@ -42438,7 +42447,7 @@
         <v>1101.2020380900001</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="47" t="s">
         <v>38</v>
       </c>
@@ -42450,7 +42459,7 @@
       <c r="H17" s="48"/>
       <c r="I17" s="48"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="49" t="s">
         <v>39</v>
       </c>
@@ -42476,7 +42485,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" ht="64" x14ac:dyDescent="0.2">
       <c r="B19" s="50" t="s">
         <v>377</v>
       </c>
@@ -42502,7 +42511,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="51" t="s">
         <v>47</v>
       </c>
@@ -42531,6 +42540,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100391E4ED4D6B5344984C5B5CBC1A28781" ma:contentTypeVersion="13" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="a8662b4a95e495bc977359cc4b8d0a5a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6218e30f-ac19-4e1a-9d42-0577826d9887" xmlns:ns3="9bef2f80-48e4-49d2-aa34-66e9d7fcf80f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b72a6a49e693c9bb3f1300811353490c" ns2:_="" ns3:_="">
     <xsd:import namespace="6218e30f-ac19-4e1a-9d42-0577826d9887"/>
@@ -42753,22 +42777,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE6C5DC3-E0D9-45E6-83DC-5991956FF726}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A0DEAC1-631B-4802-B3A4-BF232BA25A90}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29F65652-2237-4E8C-97BF-57B3390A90B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -42785,21 +42811,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE6C5DC3-E0D9-45E6-83DC-5991956FF726}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A0DEAC1-631B-4802-B3A4-BF232BA25A90}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>